<commit_message>
moved mpmdesginof to Externe Relatie Type COLLECTION
</commit_message>
<xml_diff>
--- a/admin/rdm/tw_rdm_for_prod_2021_12_08.xlsx
+++ b/admin/rdm/tw_rdm_for_prod_2021_12_08.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1164" yWindow="3624" windowWidth="27636" windowHeight="16536" firstSheet="18" activeTab="22"/>
+    <workbookView xWindow="1164" yWindow="3624" windowWidth="27636" windowHeight="16536" firstSheet="9" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Annotation lookup" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,6 @@
     <definedName name="include_codes_temp_2" localSheetId="18">'Material mapping'!$A$130:$B$143</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -5216,7 +5215,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -5362,17 +5361,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="33">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFEA9999"/>
           <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5531,6 +5549,22 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFFF0000"/>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
@@ -5622,11 +5656,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="include_codes_temp_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="include_codes_temp" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="include_codes_temp" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="include_codes_temp_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5638,11 +5672,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="include_codes_temp" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="include_codes_temp_1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="include_codes_temp_1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="include_codes_temp" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5654,11 +5688,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="include_codes_temp_2" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="include_codes_temp" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="include_codes_temp" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="include_codes_temp_2" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6291,11 +6325,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L56"/>
+  <dimension ref="A2:L55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -7007,6 +7041,21 @@
       <c r="K40" s="54"/>
       <c r="L40" s="60"/>
     </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="63" t="s">
+        <v>267</v>
+      </c>
+      <c r="B41" s="63" t="s">
+        <v>268</v>
+      </c>
+      <c r="C41" s="63"/>
+      <c r="D41" s="63" t="s">
+        <v>269</v>
+      </c>
+      <c r="E41" s="63">
+        <v>300444119</v>
+      </c>
+    </row>
     <row r="43" spans="1:12" ht="18">
       <c r="A43" s="58" t="s">
         <v>1560</v>
@@ -7150,14 +7199,14 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="19" t="s">
-        <v>267</v>
+        <v>292</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>268</v>
+        <v>293</v>
       </c>
       <c r="C53" s="19"/>
       <c r="D53" s="19" t="s">
-        <v>269</v>
+        <v>294</v>
       </c>
       <c r="E53" s="19">
         <v>300444119</v>
@@ -7166,14 +7215,14 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="19" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="C54" s="19"/>
       <c r="D54" s="19" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="E54" s="19">
         <v>300444119</v>
@@ -7182,173 +7231,177 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="19" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C55" s="19"/>
       <c r="D55" s="19" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="E55" s="19">
         <v>300444119</v>
       </c>
       <c r="F55" s="57"/>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="19" t="s">
-        <v>286</v>
-      </c>
-      <c r="B56" s="19" t="s">
-        <v>287</v>
-      </c>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19" t="s">
-        <v>288</v>
-      </c>
-      <c r="E56" s="19">
-        <v>300444119</v>
-      </c>
-      <c r="F56" s="57"/>
     </row>
   </sheetData>
   <sortState ref="A3:F28">
     <sortCondition ref="D3:D28"/>
   </sortState>
-  <conditionalFormatting sqref="B55:B56">
-    <cfRule type="expression" dxfId="28" priority="25">
-      <formula>AND(NOT(ISBLANK(B55:B988)),ISBLANK(D55:D988))</formula>
+  <conditionalFormatting sqref="B54:B55">
+    <cfRule type="expression" dxfId="32" priority="25">
+      <formula>AND(NOT(ISBLANK(B54:B987)),ISBLANK(D54:D987))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A55:A56">
-    <cfRule type="expression" dxfId="27" priority="26">
-      <formula>AND(NOT(ISBLANK(B55:B988)),ISBLANK(A55:A988))</formula>
+  <conditionalFormatting sqref="A54:A55">
+    <cfRule type="expression" dxfId="31" priority="26">
+      <formula>AND(NOT(ISBLANK(B54:B987)),ISBLANK(A54:A987))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B55:B56 D55">
-    <cfRule type="expression" dxfId="26" priority="27">
-      <formula>AND(NOT(ISBLANK(J55:J988)), J55:J988 &lt; 1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
-    <cfRule type="expression" dxfId="25" priority="1">
-      <formula>AND(NOT(ISBLANK(D56:D989)),ISBLANK(E56:E989))</formula>
+  <conditionalFormatting sqref="B54:B55 D54">
+    <cfRule type="expression" dxfId="30" priority="27">
+      <formula>AND(NOT(ISBLANK(J54:J987)), J54:J987 &lt; 1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55">
-    <cfRule type="expression" dxfId="24" priority="10">
-      <formula>AND(NOT(ISBLANK(D55:D988)),ISBLANK(F58:F988))</formula>
+    <cfRule type="expression" dxfId="29" priority="1">
+      <formula>AND(NOT(ISBLANK(D55:D988)),ISBLANK(E55:E988))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B53:B54">
-    <cfRule type="expression" dxfId="23" priority="259">
+  <conditionalFormatting sqref="D54">
+    <cfRule type="expression" dxfId="28" priority="10">
+      <formula>AND(NOT(ISBLANK(D54:D987)),ISBLANK(F57:F987))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B53">
+    <cfRule type="expression" dxfId="27" priority="259">
       <formula>AND(NOT(ISBLANK(B53:B984)),ISBLANK(D53:D984))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A53:A54">
-    <cfRule type="expression" dxfId="22" priority="261">
+  <conditionalFormatting sqref="A53">
+    <cfRule type="expression" dxfId="26" priority="261">
       <formula>AND(NOT(ISBLANK(B53:B984)),ISBLANK(A53:A984))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D53:D54 B53:B54">
-    <cfRule type="expression" dxfId="21" priority="263">
+  <conditionalFormatting sqref="D53 B53">
+    <cfRule type="expression" dxfId="25" priority="263">
       <formula>AND(NOT(ISBLANK(J53:J984)), J53:J984 &lt; 1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D53:D54">
-    <cfRule type="expression" dxfId="20" priority="301">
+  <conditionalFormatting sqref="D53">
+    <cfRule type="expression" dxfId="24" priority="301">
       <formula>AND(NOT(ISBLANK(D53:D984)),ISBLANK(F60:F984))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51:B52">
-    <cfRule type="expression" dxfId="19" priority="302">
-      <formula>AND(NOT(ISBLANK(B51:B981)),ISBLANK(D51:D981))</formula>
+    <cfRule type="expression" dxfId="21" priority="403">
+      <formula>AND(NOT(ISBLANK(B51:B980)),ISBLANK(D51:D980))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51:A52">
-    <cfRule type="expression" dxfId="18" priority="303">
-      <formula>AND(NOT(ISBLANK(B51:B981)),ISBLANK(A51:A981))</formula>
+    <cfRule type="expression" dxfId="20" priority="404">
+      <formula>AND(NOT(ISBLANK(B51:B980)),ISBLANK(A51:A980))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51:D52 B51:B52">
-    <cfRule type="expression" dxfId="17" priority="304">
-      <formula>AND(NOT(ISBLANK(J51:J981)), J51:J981 &lt; 1)</formula>
+    <cfRule type="expression" dxfId="19" priority="405">
+      <formula>AND(NOT(ISBLANK(J51:J980)), J51:J980 &lt; 1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51:D52">
-    <cfRule type="expression" dxfId="16" priority="306">
-      <formula>AND(NOT(ISBLANK(D51:D981)),ISBLANK(F58:F981))</formula>
+    <cfRule type="expression" dxfId="18" priority="407">
+      <formula>AND(NOT(ISBLANK(D51:D980)),ISBLANK(F57:F980))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49:B50">
-    <cfRule type="expression" dxfId="15" priority="341">
-      <formula>AND(NOT(ISBLANK(B49:B974)),ISBLANK(D49:D974))</formula>
+    <cfRule type="expression" dxfId="17" priority="408">
+      <formula>AND(NOT(ISBLANK(B49:B973)),ISBLANK(D49:D973))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:A50">
-    <cfRule type="expression" dxfId="14" priority="342">
-      <formula>AND(NOT(ISBLANK(B49:B974)),ISBLANK(A49:A974))</formula>
+    <cfRule type="expression" dxfId="16" priority="409">
+      <formula>AND(NOT(ISBLANK(B49:B973)),ISBLANK(A49:A973))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49:D50 B49:B50">
-    <cfRule type="expression" dxfId="13" priority="343">
-      <formula>AND(NOT(ISBLANK(J49:J974)), J49:J974 &lt; 1)</formula>
+    <cfRule type="expression" dxfId="15" priority="410">
+      <formula>AND(NOT(ISBLANK(J49:J973)), J49:J973 &lt; 1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49:D50">
-    <cfRule type="expression" dxfId="12" priority="345">
-      <formula>AND(NOT(ISBLANK(D49:D974)),ISBLANK(F57:F974))</formula>
+    <cfRule type="expression" dxfId="14" priority="412">
+      <formula>AND(NOT(ISBLANK(D49:D973)),ISBLANK(F56:F973))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D8 D10 D15:D16 D23 D26 D45:D48">
-    <cfRule type="expression" dxfId="11" priority="371">
-      <formula>AND(NOT(ISBLANK(D4:D926)),ISBLANK(E4:E926))</formula>
+    <cfRule type="expression" dxfId="13" priority="413">
+      <formula>AND(NOT(ISBLANK(D4:D925)),ISBLANK(E4:E925))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B26 B45:B48">
-    <cfRule type="expression" dxfId="10" priority="377">
-      <formula>AND(NOT(ISBLANK(B4:B926)),ISBLANK(D4:D926))</formula>
+    <cfRule type="expression" dxfId="12" priority="419">
+      <formula>AND(NOT(ISBLANK(B4:B925)),ISBLANK(D4:D925))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A26 A45:A48">
-    <cfRule type="expression" dxfId="9" priority="379">
-      <formula>AND(NOT(ISBLANK(B4:B926)),ISBLANK(A4:A926))</formula>
+    <cfRule type="expression" dxfId="11" priority="421">
+      <formula>AND(NOT(ISBLANK(B4:B925)),ISBLANK(A4:A925))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B26 D9 D11:D14 D17:D22 D24:D25 B45:B48">
-    <cfRule type="expression" dxfId="8" priority="381">
-      <formula>AND(NOT(ISBLANK(J4:J926)), J4:J926 &lt; 1)</formula>
+    <cfRule type="expression" dxfId="10" priority="423">
+      <formula>AND(NOT(ISBLANK(J4:J925)), J4:J925 &lt; 1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="expression" dxfId="7" priority="387">
-      <formula>AND(NOT(ISBLANK(D9:D931)),ISBLANK(F27:F931))</formula>
+    <cfRule type="expression" dxfId="9" priority="429">
+      <formula>AND(NOT(ISBLANK(D9:D930)),ISBLANK(F27:F930))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11:D13">
-    <cfRule type="expression" dxfId="6" priority="388">
-      <formula>AND(NOT(ISBLANK(D11:D933)),ISBLANK(F27:F933))</formula>
+    <cfRule type="expression" dxfId="8" priority="430">
+      <formula>AND(NOT(ISBLANK(D11:D932)),ISBLANK(F27:F932))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="5" priority="389">
-      <formula>AND(NOT(ISBLANK(D14:D936)),ISBLANK(F29:F936))</formula>
+    <cfRule type="expression" dxfId="7" priority="431">
+      <formula>AND(NOT(ISBLANK(D14:D935)),ISBLANK(F29:F935))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17:D19">
-    <cfRule type="expression" dxfId="4" priority="390">
-      <formula>AND(NOT(ISBLANK(D17:D939)),ISBLANK(F27:F939))</formula>
+    <cfRule type="expression" dxfId="6" priority="432">
+      <formula>AND(NOT(ISBLANK(D17:D938)),ISBLANK(F27:F938))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20:D22">
-    <cfRule type="expression" dxfId="3" priority="391">
-      <formula>AND(NOT(ISBLANK(D20:D942)),ISBLANK(F29:F942))</formula>
+    <cfRule type="expression" dxfId="5" priority="433">
+      <formula>AND(NOT(ISBLANK(D20:D941)),ISBLANK(F29:F941))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:D25">
-    <cfRule type="expression" dxfId="2" priority="392">
-      <formula>AND(NOT(ISBLANK(D24:D946)),ISBLANK(F27:F946))</formula>
+    <cfRule type="expression" dxfId="4" priority="434">
+      <formula>AND(NOT(ISBLANK(D24:D945)),ISBLANK(F27:F945))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B41">
+    <cfRule type="expression" dxfId="3" priority="435">
+      <formula>AND(NOT(ISBLANK(B41:B983)),ISBLANK(D41:D983))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41">
+    <cfRule type="expression" dxfId="2" priority="436">
+      <formula>AND(NOT(ISBLANK(B41:B983)),ISBLANK(A41:A983))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41 B41">
+    <cfRule type="expression" dxfId="1" priority="437">
+      <formula>AND(NOT(ISBLANK(J53:J983)), J53:J983 &lt; 1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="expression" dxfId="0" priority="439">
+      <formula>AND(NOT(ISBLANK(D41:D983)),ISBLANK(F59:F983))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12228,12 +12281,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>AND(NOT(ISBLANK(B16:B1143)),ISBLANK(D16:D1143))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="0" priority="9">
+    <cfRule type="expression" dxfId="22" priority="9">
       <formula>AND(NOT(ISBLANK(#REF!)), #REF! &lt; 1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16822,7 +16875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+    <sheetView topLeftCell="A139" workbookViewId="0">
       <selection activeCell="F142" sqref="F142"/>
     </sheetView>
   </sheetViews>

</xml_diff>